<commit_message>
added excel table creater classes
</commit_message>
<xml_diff>
--- a/resources/reports/analysisDoc.xlsx
+++ b/resources/reports/analysisDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,46 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>year-month-date</t>
-  </si>
-  <si>
-    <t>total buying amount</t>
-  </si>
-  <si>
-    <t>total buying quantity</t>
-  </si>
-  <si>
-    <t>total selling profit</t>
-  </si>
-  <si>
-    <t>total selling cast</t>
-  </si>
-  <si>
-    <t>total selling quantity</t>
-  </si>
-  <si>
-    <t>total selling amount</t>
-  </si>
-  <si>
-    <t>total buying cast</t>
-  </si>
-  <si>
-    <t>expected profit</t>
-  </si>
-  <si>
-    <t>available itams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analysis for </t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,59 +32,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF66FF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99FF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -126,100 +49,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,72 +363,7 @@
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>